<commit_message>
pretrained model for 100 sentences
</commit_message>
<xml_diff>
--- a/train/results.xlsx
+++ b/train/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Antoine/training_ML/transformer/train/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A77E63-6F5E-0545-8801-6478F3CBA55A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9871D01B-31ED-BF46-816B-3C4ED205F721}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{E5EF0A20-FAE9-8841-B3FF-3D9ABDE29D44}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Hardware</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>europarl</t>
+  </si>
+  <si>
+    <t>Macbook</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DB81ED-E744-E848-B570-5B80FBCE336F}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,77 +567,90 @@
         <v>26</v>
       </c>
       <c r="B2" s="2">
-        <v>100000</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="E2" s="2">
         <v>0.19</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.91</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G2" s="2">
-        <f>480/B2</f>
-        <v>4.7999999999999996E-3</v>
+        <f>10/B2</f>
+        <v>0.1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2">
         <v>1000000</v>
       </c>
       <c r="J2" s="2">
-        <v>32215</v>
+        <v>1013</v>
       </c>
       <c r="K2" s="2">
-        <v>12</v>
+        <v>0.06</v>
       </c>
       <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
         <v>2</v>
       </c>
-      <c r="M2" s="2">
-        <v>4</v>
-      </c>
       <c r="N2" s="2">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2">
-        <v>1024</v>
+        <v>128</v>
       </c>
       <c r="P2" s="2">
         <f>((B2*S2)/U2)*T2</f>
-        <v>450000</v>
+        <v>8000</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="R2" s="2">
-        <v>16000</v>
+        <v>1000</v>
       </c>
       <c r="S2" s="2">
         <v>0.8</v>
       </c>
       <c r="T2" s="2">
-        <v>450</v>
+        <v>1000</v>
       </c>
       <c r="U2" s="2">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="V2" s="2">
-        <v>160</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="3">
-        <v>1000000</v>
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.55000000000000004</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="G3" s="2">
+        <f>480/B3</f>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>13</v>
@@ -642,8 +658,14 @@
       <c r="I3" s="2">
         <v>1000000</v>
       </c>
-      <c r="L3" s="3">
-        <v>6</v>
+      <c r="J3" s="2">
+        <v>32215</v>
+      </c>
+      <c r="K3" s="2">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2</v>
       </c>
       <c r="M3" s="2">
         <v>4</v>
@@ -654,6 +676,10 @@
       <c r="O3" s="2">
         <v>1024</v>
       </c>
+      <c r="P3" s="2">
+        <f>((B3*S3)/U3)*T3</f>
+        <v>450000</v>
+      </c>
       <c r="Q3" s="2" t="s">
         <v>21</v>
       </c>
@@ -663,14 +689,57 @@
       <c r="S3" s="2">
         <v>0.8</v>
       </c>
-      <c r="U3" s="3">
+      <c r="T3" s="2">
+        <v>450</v>
+      </c>
+      <c r="U3" s="2">
+        <v>80</v>
+      </c>
+      <c r="V3" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="L4" s="3">
+        <v>6</v>
+      </c>
+      <c r="M4" s="2">
+        <v>4</v>
+      </c>
+      <c r="N4" s="2">
+        <v>256</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1024</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="2">
+        <v>16000</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U4" s="3">
         <v>40</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V4" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -680,13 +749,14 @@
     <row r="11" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+    <row r="14" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
     </row>
-    <row r="15" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>